<commit_message>
Arquivos Metodologia + Diagramas
</commit_message>
<xml_diff>
--- a/ExecucoesGerais/ParametrosLivres.xlsx
+++ b/ExecucoesGerais/ParametrosLivres.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14460" windowHeight="7935" firstSheet="2" activeTab="3"/>
+    <workbookView windowWidth="19485" windowHeight="7980" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ParamLivres" sheetId="1" r:id="rId1"/>
@@ -120,21 +120,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="26">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -154,7 +147,7 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -165,15 +158,15 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="12"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -187,8 +180,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -209,16 +203,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -240,16 +250,23 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -263,8 +280,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -277,9 +302,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -287,37 +311,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -332,7 +325,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -350,13 +427,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -368,55 +451,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -428,55 +469,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -494,7 +487,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -504,18 +509,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="56">
     <border>
@@ -527,13 +520,13 @@
     </border>
     <border>
       <left style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
         <color theme="0"/>
       </right>
       <top style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
         <color theme="0"/>
@@ -546,7 +539,7 @@
       </left>
       <right/>
       <top style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
         <color theme="0"/>
@@ -555,7 +548,7 @@
     </border>
     <border>
       <left style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
         <color theme="0"/>
@@ -564,7 +557,7 @@
         <color theme="0"/>
       </top>
       <bottom style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -577,13 +570,13 @@
         <color theme="0"/>
       </top>
       <bottom style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
         <color theme="0"/>
@@ -611,13 +604,13 @@
     </border>
     <border>
       <left style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
         <color theme="0"/>
@@ -626,16 +619,16 @@
     </border>
     <border>
       <left style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
         <color theme="0"/>
       </right>
       <top style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -647,38 +640,38 @@
         <color theme="0"/>
       </right>
       <top style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
         <color theme="0"/>
       </top>
       <bottom style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
         <color theme="0"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -691,7 +684,7 @@
       </right>
       <top/>
       <bottom style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -703,7 +696,7 @@
         <color theme="0"/>
       </right>
       <top style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
         <color theme="0"/>
@@ -712,10 +705,10 @@
     </border>
     <border>
       <left style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
         <color theme="0"/>
@@ -751,7 +744,7 @@
         <color theme="0"/>
       </top>
       <bottom style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -760,13 +753,13 @@
         <color theme="0"/>
       </left>
       <right style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -775,11 +768,11 @@
         <color theme="0"/>
       </left>
       <right style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -788,10 +781,10 @@
         <color theme="0"/>
       </left>
       <right style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
         <color theme="0"/>
@@ -803,7 +796,7 @@
         <color theme="0"/>
       </left>
       <right style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
         <color theme="0"/>
@@ -818,141 +811,141 @@
         <color theme="0"/>
       </left>
       <right style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
         <color theme="0"/>
       </top>
       <bottom style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -960,48 +953,48 @@
     <border>
       <left/>
       <right style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1009,23 +1002,23 @@
       <left/>
       <right/>
       <top style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1033,7 +1026,7 @@
       <left/>
       <right/>
       <top style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -1041,20 +1034,20 @@
     <border>
       <left/>
       <right style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -1063,7 +1056,7 @@
     <border>
       <left/>
       <right style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -1074,24 +1067,24 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -1100,53 +1093,86 @@
     </border>
     <border>
       <left style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="medium">
-        <color auto="true"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color auto="true"/>
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1166,15 +1192,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1190,50 +1207,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1248,443 +1221,490 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="54" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="53" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="52" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="50" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="48" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="48" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="49" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="51" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="51" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="31" borderId="55" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="55" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="54" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="48" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="52" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="51" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="51" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="50" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="49" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="49" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="53" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
-      <alignment vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="30" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1866,7 +1886,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1890,9 +1910,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1916,7 +1936,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -1969,7 +1989,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1994,7 +2014,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -2014,321 +2034,321 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="1.24166666666667" customWidth="true"/>
-    <col min="2" max="2" width="10.375" customWidth="true"/>
-    <col min="3" max="3" width="12.75" customWidth="true"/>
+    <col min="1" max="1" width="1.24166666666667" customWidth="1"/>
+    <col min="2" max="2" width="10.375" customWidth="1"/>
+    <col min="3" max="3" width="12.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="9" customHeight="true"/>
+    <row r="1" ht="9" customHeight="1"/>
     <row r="2" spans="2:7">
-      <c r="B2" s="93" t="s">
+      <c r="B2" s="102" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="93"/>
-      <c r="F2" s="93"/>
-      <c r="G2" s="93"/>
+      <c r="C2" s="102"/>
+      <c r="D2" s="102" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="102"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="102"/>
     </row>
     <row r="3" spans="2:7">
-      <c r="B3" s="93"/>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93" t="s">
+      <c r="B3" s="102"/>
+      <c r="C3" s="102"/>
+      <c r="D3" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="93" t="s">
+      <c r="E3" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="93" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="93" t="s">
+      <c r="F3" s="102" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="102" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:7">
-      <c r="B4" s="93" t="s">
+      <c r="B4" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="93" t="s">
+      <c r="C4" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="93" t="s">
+      <c r="D4" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="93"/>
-      <c r="F4" s="93"/>
-      <c r="G4" s="93"/>
+      <c r="E4" s="102"/>
+      <c r="F4" s="102"/>
+      <c r="G4" s="102"/>
     </row>
     <row r="5" spans="2:7">
-      <c r="B5" s="93"/>
-      <c r="C5" s="93" t="s">
+      <c r="B5" s="102"/>
+      <c r="C5" s="102" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="93" t="s">
+      <c r="D5" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="93"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="93"/>
+      <c r="E5" s="102"/>
+      <c r="F5" s="102"/>
+      <c r="G5" s="102"/>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="93"/>
-      <c r="C6" s="93" t="s">
+      <c r="B6" s="102"/>
+      <c r="C6" s="102" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="93"/>
-      <c r="E6" s="93"/>
-      <c r="F6" s="93"/>
-      <c r="G6" s="93"/>
+      <c r="D6" s="102"/>
+      <c r="E6" s="102"/>
+      <c r="F6" s="102"/>
+      <c r="G6" s="102"/>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="93"/>
-      <c r="C7" s="93" t="s">
+      <c r="B7" s="102"/>
+      <c r="C7" s="102" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="93"/>
-      <c r="E7" s="93"/>
-      <c r="F7" s="93"/>
-      <c r="G7" s="93"/>
+      <c r="D7" s="102"/>
+      <c r="E7" s="102"/>
+      <c r="F7" s="102"/>
+      <c r="G7" s="102"/>
     </row>
     <row r="8" spans="2:7">
-      <c r="B8" s="93"/>
-      <c r="C8" s="93" t="s">
+      <c r="B8" s="102"/>
+      <c r="C8" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="93"/>
-      <c r="E8" s="93"/>
-      <c r="F8" s="93"/>
-      <c r="G8" s="93"/>
+      <c r="D8" s="102"/>
+      <c r="E8" s="102"/>
+      <c r="F8" s="102"/>
+      <c r="G8" s="102"/>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="93"/>
-      <c r="C9" s="93" t="s">
+      <c r="B9" s="102"/>
+      <c r="C9" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="93"/>
-      <c r="E9" s="93"/>
-      <c r="F9" s="93"/>
-      <c r="G9" s="93"/>
+      <c r="D9" s="102"/>
+      <c r="E9" s="102"/>
+      <c r="F9" s="102"/>
+      <c r="G9" s="102"/>
     </row>
     <row r="10" spans="2:7">
-      <c r="B10" s="93" t="s">
+      <c r="B10" s="102" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="93" t="s">
+      <c r="C10" s="102" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="93" t="s">
+      <c r="D10" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="93" t="s">
+      <c r="E10" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="93"/>
-      <c r="G10" s="93"/>
+      <c r="F10" s="102"/>
+      <c r="G10" s="102"/>
     </row>
     <row r="11" spans="2:7">
-      <c r="B11" s="93"/>
-      <c r="C11" s="93" t="s">
+      <c r="B11" s="102"/>
+      <c r="C11" s="102" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="93"/>
-      <c r="E11" s="93" t="s">
+      <c r="D11" s="102"/>
+      <c r="E11" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="93"/>
-      <c r="G11" s="93"/>
+      <c r="F11" s="102"/>
+      <c r="G11" s="102"/>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="93"/>
-      <c r="C12" s="93" t="s">
+      <c r="B12" s="102"/>
+      <c r="C12" s="102" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="93"/>
-      <c r="E12" s="93" t="s">
+      <c r="D12" s="102"/>
+      <c r="E12" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="93"/>
-      <c r="G12" s="93"/>
+      <c r="F12" s="102"/>
+      <c r="G12" s="102"/>
     </row>
     <row r="13" spans="2:7">
-      <c r="B13" s="93"/>
-      <c r="C13" s="93" t="s">
+      <c r="B13" s="102"/>
+      <c r="C13" s="102" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="93" t="s">
+      <c r="D13" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="93" t="s">
+      <c r="E13" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="F13" s="93" t="s">
+      <c r="F13" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="G13" s="93" t="s">
+      <c r="G13" s="102" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="2:7">
-      <c r="B14" s="93"/>
-      <c r="C14" s="93" t="s">
+      <c r="B14" s="102"/>
+      <c r="C14" s="102" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="93"/>
-      <c r="E14" s="93" t="s">
+      <c r="D14" s="102"/>
+      <c r="E14" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="93" t="s">
+      <c r="F14" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="93" t="s">
+      <c r="G14" s="102" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="15" spans="2:7">
-      <c r="B15" s="93"/>
-      <c r="C15" s="93" t="s">
+      <c r="B15" s="102"/>
+      <c r="C15" s="102" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="93"/>
-      <c r="E15" s="93" t="s">
+      <c r="D15" s="102"/>
+      <c r="E15" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="F15" s="93" t="s">
+      <c r="F15" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="93" t="s">
+      <c r="G15" s="102" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="18" spans="2:7">
-      <c r="B18" s="93" t="s">
+      <c r="B18" s="102" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="93"/>
-      <c r="D18" s="93" t="s">
-        <v>1</v>
-      </c>
-      <c r="E18" s="93"/>
-      <c r="F18" s="93"/>
-      <c r="G18" s="93"/>
+      <c r="C18" s="102"/>
+      <c r="D18" s="102" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="102"/>
+      <c r="F18" s="102"/>
+      <c r="G18" s="102"/>
     </row>
     <row r="19" spans="2:7">
-      <c r="B19" s="93"/>
-      <c r="C19" s="93"/>
-      <c r="D19" s="93" t="s">
+      <c r="B19" s="102"/>
+      <c r="C19" s="102"/>
+      <c r="D19" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="E19" s="93" t="s">
+      <c r="E19" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="F19" s="93" t="s">
-        <v>4</v>
-      </c>
-      <c r="G19" s="93" t="s">
+      <c r="F19" s="102" t="s">
+        <v>4</v>
+      </c>
+      <c r="G19" s="102" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="2:7">
-      <c r="B20" s="93" t="s">
+      <c r="B20" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="93" t="s">
+      <c r="C20" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="93" t="s">
+      <c r="D20" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="93"/>
-      <c r="F20" s="93"/>
-      <c r="G20" s="93"/>
+      <c r="E20" s="102"/>
+      <c r="F20" s="102"/>
+      <c r="G20" s="102"/>
     </row>
     <row r="21" spans="2:7">
-      <c r="B21" s="93"/>
-      <c r="C21" s="93" t="s">
+      <c r="B21" s="102"/>
+      <c r="C21" s="102" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="93" t="s">
+      <c r="D21" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="93"/>
-      <c r="F21" s="93"/>
-      <c r="G21" s="93"/>
+      <c r="E21" s="102"/>
+      <c r="F21" s="102"/>
+      <c r="G21" s="102"/>
     </row>
     <row r="22" spans="2:7">
-      <c r="B22" s="93"/>
-      <c r="C22" s="93" t="s">
+      <c r="B22" s="102"/>
+      <c r="C22" s="102" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="93"/>
-      <c r="E22" s="93"/>
-      <c r="F22" s="93"/>
-      <c r="G22" s="93"/>
+      <c r="D22" s="102"/>
+      <c r="E22" s="102"/>
+      <c r="F22" s="102"/>
+      <c r="G22" s="102"/>
     </row>
     <row r="23" spans="2:7">
-      <c r="B23" s="93"/>
-      <c r="C23" s="93" t="s">
+      <c r="B23" s="102"/>
+      <c r="C23" s="102" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="93"/>
-      <c r="E23" s="93"/>
-      <c r="F23" s="93"/>
-      <c r="G23" s="93"/>
+      <c r="D23" s="102"/>
+      <c r="E23" s="102"/>
+      <c r="F23" s="102"/>
+      <c r="G23" s="102"/>
     </row>
     <row r="24" spans="2:7">
-      <c r="B24" s="93"/>
-      <c r="C24" s="93" t="s">
+      <c r="B24" s="102"/>
+      <c r="C24" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="93"/>
-      <c r="E24" s="93"/>
-      <c r="F24" s="93"/>
-      <c r="G24" s="93"/>
+      <c r="D24" s="102"/>
+      <c r="E24" s="102"/>
+      <c r="F24" s="102"/>
+      <c r="G24" s="102"/>
     </row>
     <row r="25" spans="2:7">
-      <c r="B25" s="93"/>
-      <c r="C25" s="93" t="s">
+      <c r="B25" s="102"/>
+      <c r="C25" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="93"/>
-      <c r="E25" s="93"/>
-      <c r="F25" s="93"/>
-      <c r="G25" s="93"/>
+      <c r="D25" s="102"/>
+      <c r="E25" s="102"/>
+      <c r="F25" s="102"/>
+      <c r="G25" s="102"/>
     </row>
     <row r="26" spans="2:7">
-      <c r="B26" s="94" t="s">
+      <c r="B26" s="103" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="93" t="s">
+      <c r="C26" s="102" t="s">
         <v>15</v>
       </c>
-      <c r="D26" s="93" t="s">
+      <c r="D26" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="E26" s="93" t="s">
+      <c r="E26" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="F26" s="93"/>
-      <c r="G26" s="93"/>
+      <c r="F26" s="102"/>
+      <c r="G26" s="102"/>
     </row>
     <row r="27" spans="2:7">
-      <c r="B27" s="95"/>
-      <c r="C27" s="93" t="s">
+      <c r="B27" s="104"/>
+      <c r="C27" s="102" t="s">
         <v>18</v>
       </c>
-      <c r="D27" s="93" t="s">
+      <c r="D27" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="93" t="s">
+      <c r="E27" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="F27" s="93" t="s">
+      <c r="F27" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="G27" s="93" t="s">
+      <c r="G27" s="102" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2359,718 +2379,718 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="1.375" customWidth="true"/>
-    <col min="3" max="3" width="7.25" customWidth="true"/>
-    <col min="5" max="5" width="10" customWidth="true"/>
-    <col min="6" max="6" width="5.625" customWidth="true"/>
-    <col min="7" max="7" width="8.25" customWidth="true"/>
-    <col min="8" max="9" width="9.625" customWidth="true"/>
-    <col min="10" max="13" width="12.75" customWidth="true"/>
+    <col min="2" max="2" width="1.375" customWidth="1"/>
+    <col min="3" max="3" width="7.25" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="5.625" customWidth="1"/>
+    <col min="7" max="7" width="8.25" customWidth="1"/>
+    <col min="8" max="9" width="9.625" customWidth="1"/>
+    <col min="10" max="13" width="12.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="9" customHeight="true" spans="6:9">
+    <row r="1" ht="9" customHeight="1" spans="6:9">
       <c r="F1" s="12"/>
       <c r="G1" s="12"/>
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
     </row>
     <row r="2" ht="15" spans="3:13">
-      <c r="C2" s="56" t="s">
+      <c r="C2" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="57"/>
-      <c r="E2" s="68" t="s">
+      <c r="D2" s="66"/>
+      <c r="E2" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="69" t="s">
+      <c r="F2" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="70"/>
-      <c r="H2" s="71" t="s">
+      <c r="G2" s="79"/>
+      <c r="H2" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="76"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="76"/>
-      <c r="L2" s="76"/>
-      <c r="M2" s="77"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="86"/>
     </row>
     <row r="3" ht="15" spans="3:13">
-      <c r="C3" s="58"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="73" t="s">
+      <c r="C3" s="67"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="74" t="s">
+      <c r="G3" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="73" t="s">
+      <c r="H3" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="73" t="s">
+      <c r="I3" s="82" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="73" t="s">
+      <c r="J3" s="82" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="73" t="s">
+      <c r="K3" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="73" t="s">
+      <c r="L3" s="82" t="s">
         <v>19</v>
       </c>
-      <c r="M3" s="74" t="s">
+      <c r="M3" s="83" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="2:13">
       <c r="B4" s="5"/>
-      <c r="C4" s="60" t="s">
+      <c r="C4" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="61"/>
-      <c r="E4" s="75" t="s">
+      <c r="D4" s="70"/>
+      <c r="E4" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="76">
+      <c r="F4" s="85">
         <v>1.25</v>
       </c>
-      <c r="G4" s="77">
+      <c r="G4" s="86">
         <v>2.75</v>
       </c>
-      <c r="H4" s="78">
+      <c r="H4" s="87">
         <v>1.5</v>
       </c>
-      <c r="I4" s="78">
+      <c r="I4" s="87">
         <v>3</v>
       </c>
-      <c r="J4" s="78" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" s="78" t="s">
-        <v>25</v>
-      </c>
-      <c r="L4" s="78" t="s">
-        <v>25</v>
-      </c>
-      <c r="M4" s="90" t="s">
+      <c r="J4" s="87" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="87" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" s="87" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" s="99" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="5" spans="2:13">
       <c r="B5" s="5"/>
-      <c r="C5" s="62"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="79" t="s">
+      <c r="C5" s="71"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="80" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="81" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="78">
+      <c r="F5" s="89" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="90" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="87">
         <v>0.8</v>
       </c>
-      <c r="I5" s="78">
-        <v>1</v>
-      </c>
-      <c r="J5" s="78">
+      <c r="I5" s="87">
+        <v>1</v>
+      </c>
+      <c r="J5" s="87">
         <v>0.8</v>
       </c>
-      <c r="K5" s="78">
-        <v>1</v>
-      </c>
-      <c r="L5" s="78">
-        <v>1</v>
-      </c>
-      <c r="M5" s="90">
+      <c r="K5" s="87">
+        <v>1</v>
+      </c>
+      <c r="L5" s="87">
+        <v>1</v>
+      </c>
+      <c r="M5" s="99">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:13">
       <c r="B6" s="5"/>
-      <c r="C6" s="62"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="79" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="80" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="81" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" s="78" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" s="78">
-        <v>4</v>
-      </c>
-      <c r="J6" s="78" t="s">
-        <v>25</v>
-      </c>
-      <c r="K6" s="78" t="s">
-        <v>25</v>
-      </c>
-      <c r="L6" s="78">
-        <v>4</v>
-      </c>
-      <c r="M6" s="90">
+      <c r="C6" s="71"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="88" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="89" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="90" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="87" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="87">
+        <v>4</v>
+      </c>
+      <c r="J6" s="87" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" s="87" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" s="87">
+        <v>4</v>
+      </c>
+      <c r="M6" s="99">
         <v>4</v>
       </c>
     </row>
     <row r="7" ht="15" spans="2:13">
       <c r="B7" s="5"/>
-      <c r="C7" s="64"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="82" t="s">
+      <c r="C7" s="73"/>
+      <c r="D7" s="74"/>
+      <c r="E7" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="83" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" s="84" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="78" t="s">
-        <v>25</v>
-      </c>
-      <c r="I7" s="78">
-        <v>1</v>
-      </c>
-      <c r="J7" s="89" t="s">
-        <v>25</v>
-      </c>
-      <c r="K7" s="89" t="s">
-        <v>25</v>
-      </c>
-      <c r="L7" s="78">
-        <v>1</v>
-      </c>
-      <c r="M7" s="90">
+      <c r="F7" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="93" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="87" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="87">
+        <v>1</v>
+      </c>
+      <c r="J7" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" s="87">
+        <v>1</v>
+      </c>
+      <c r="M7" s="99">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:13">
       <c r="B8" s="5"/>
-      <c r="C8" s="66" t="s">
+      <c r="C8" s="75" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="67"/>
-      <c r="E8" s="75" t="s">
+      <c r="D8" s="76"/>
+      <c r="E8" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="76">
-        <v>1</v>
-      </c>
-      <c r="G8" s="77">
+      <c r="F8" s="85">
+        <v>1</v>
+      </c>
+      <c r="G8" s="86">
         <v>1.75</v>
       </c>
-      <c r="H8" s="85">
+      <c r="H8" s="94">
         <v>1.5</v>
       </c>
-      <c r="I8" s="88">
-        <v>4</v>
-      </c>
-      <c r="J8" s="88" t="s">
-        <v>25</v>
-      </c>
-      <c r="K8" s="88" t="s">
-        <v>25</v>
-      </c>
-      <c r="L8" s="88" t="s">
-        <v>25</v>
-      </c>
-      <c r="M8" s="91" t="s">
+      <c r="I8" s="97">
+        <v>4</v>
+      </c>
+      <c r="J8" s="97" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" s="97" t="s">
+        <v>25</v>
+      </c>
+      <c r="L8" s="97" t="s">
+        <v>25</v>
+      </c>
+      <c r="M8" s="100" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="9" spans="2:13">
       <c r="B9" s="5"/>
-      <c r="C9" s="62"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="79" t="s">
+      <c r="C9" s="71"/>
+      <c r="D9" s="72"/>
+      <c r="E9" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="80" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="81" t="s">
-        <v>25</v>
-      </c>
-      <c r="H9" s="86">
+      <c r="F9" s="89" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="90" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="95">
         <v>1.2</v>
       </c>
-      <c r="I9" s="78">
-        <v>1</v>
-      </c>
-      <c r="J9" s="78">
+      <c r="I9" s="87">
+        <v>1</v>
+      </c>
+      <c r="J9" s="87">
         <v>0.8</v>
       </c>
-      <c r="K9" s="78">
-        <v>1</v>
-      </c>
-      <c r="L9" s="78">
-        <v>1</v>
-      </c>
-      <c r="M9" s="90">
+      <c r="K9" s="87">
+        <v>1</v>
+      </c>
+      <c r="L9" s="87">
+        <v>1</v>
+      </c>
+      <c r="M9" s="99">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:13">
       <c r="B10" s="5"/>
-      <c r="C10" s="62"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="79" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10" s="80" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" s="81" t="s">
-        <v>25</v>
-      </c>
-      <c r="H10" s="86" t="s">
-        <v>25</v>
-      </c>
-      <c r="I10" s="78">
-        <v>4</v>
-      </c>
-      <c r="J10" s="78" t="s">
-        <v>25</v>
-      </c>
-      <c r="K10" s="78" t="s">
-        <v>25</v>
-      </c>
-      <c r="L10" s="78">
-        <v>4</v>
-      </c>
-      <c r="M10" s="90">
+      <c r="C10" s="71"/>
+      <c r="D10" s="72"/>
+      <c r="E10" s="88" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="89" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="90" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="95" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" s="87">
+        <v>4</v>
+      </c>
+      <c r="J10" s="87" t="s">
+        <v>25</v>
+      </c>
+      <c r="K10" s="87" t="s">
+        <v>25</v>
+      </c>
+      <c r="L10" s="87">
+        <v>4</v>
+      </c>
+      <c r="M10" s="99">
         <v>4</v>
       </c>
     </row>
     <row r="11" ht="15" spans="2:13">
       <c r="B11" s="5"/>
-      <c r="C11" s="64"/>
-      <c r="D11" s="65"/>
-      <c r="E11" s="82" t="s">
+      <c r="C11" s="73"/>
+      <c r="D11" s="74"/>
+      <c r="E11" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="83" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" s="84" t="s">
-        <v>25</v>
-      </c>
-      <c r="H11" s="87" t="s">
-        <v>25</v>
-      </c>
-      <c r="I11" s="89">
-        <v>1</v>
-      </c>
-      <c r="J11" s="89" t="s">
-        <v>25</v>
-      </c>
-      <c r="K11" s="89" t="s">
-        <v>25</v>
-      </c>
-      <c r="L11" s="89">
-        <v>1</v>
-      </c>
-      <c r="M11" s="92">
+      <c r="F11" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="93" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" s="98">
+        <v>1</v>
+      </c>
+      <c r="J11" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="L11" s="98">
+        <v>1</v>
+      </c>
+      <c r="M11" s="101">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:13">
       <c r="B12" s="5"/>
-      <c r="C12" s="66" t="s">
+      <c r="C12" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="67"/>
-      <c r="E12" s="75" t="s">
+      <c r="D12" s="76"/>
+      <c r="E12" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="76">
+      <c r="F12" s="85">
         <v>1.25</v>
       </c>
-      <c r="G12" s="77">
+      <c r="G12" s="86">
         <v>1.5</v>
       </c>
-      <c r="H12" s="88">
-        <v>4</v>
-      </c>
-      <c r="I12" s="88">
+      <c r="H12" s="97">
+        <v>4</v>
+      </c>
+      <c r="I12" s="97">
         <v>5</v>
       </c>
-      <c r="J12" s="78" t="s">
-        <v>25</v>
-      </c>
-      <c r="K12" s="78" t="s">
-        <v>25</v>
-      </c>
-      <c r="L12" s="78" t="s">
-        <v>25</v>
-      </c>
-      <c r="M12" s="90" t="s">
+      <c r="J12" s="87" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12" s="87" t="s">
+        <v>25</v>
+      </c>
+      <c r="L12" s="87" t="s">
+        <v>25</v>
+      </c>
+      <c r="M12" s="99" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="13" spans="2:13">
       <c r="B13" s="5"/>
-      <c r="C13" s="62"/>
-      <c r="D13" s="63"/>
-      <c r="E13" s="79" t="s">
+      <c r="C13" s="71"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="80" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="81" t="s">
-        <v>25</v>
-      </c>
-      <c r="H13" s="78">
+      <c r="F13" s="89" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="90" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="87">
         <v>2.2</v>
       </c>
-      <c r="I13" s="78">
-        <v>1</v>
-      </c>
-      <c r="J13" s="78">
+      <c r="I13" s="87">
+        <v>1</v>
+      </c>
+      <c r="J13" s="87">
         <v>1.6</v>
       </c>
-      <c r="K13" s="78">
+      <c r="K13" s="87">
         <v>1.8</v>
       </c>
-      <c r="L13" s="78">
+      <c r="L13" s="87">
         <v>2</v>
       </c>
-      <c r="M13" s="90">
+      <c r="M13" s="99">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="2:13">
       <c r="B14" s="5"/>
-      <c r="C14" s="62"/>
-      <c r="D14" s="63"/>
-      <c r="E14" s="79" t="s">
-        <v>4</v>
-      </c>
-      <c r="F14" s="80" t="s">
-        <v>25</v>
-      </c>
-      <c r="G14" s="81" t="s">
-        <v>25</v>
-      </c>
-      <c r="H14" s="78" t="s">
-        <v>25</v>
-      </c>
-      <c r="I14" s="78">
-        <v>4</v>
-      </c>
-      <c r="J14" s="78" t="s">
-        <v>25</v>
-      </c>
-      <c r="K14" s="78" t="s">
-        <v>25</v>
-      </c>
-      <c r="L14" s="78">
+      <c r="C14" s="71"/>
+      <c r="D14" s="72"/>
+      <c r="E14" s="88" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="89" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="90" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14" s="87" t="s">
+        <v>25</v>
+      </c>
+      <c r="I14" s="87">
+        <v>4</v>
+      </c>
+      <c r="J14" s="87" t="s">
+        <v>25</v>
+      </c>
+      <c r="K14" s="87" t="s">
+        <v>25</v>
+      </c>
+      <c r="L14" s="87">
         <v>8</v>
       </c>
-      <c r="M14" s="90">
+      <c r="M14" s="99">
         <v>4</v>
       </c>
     </row>
     <row r="15" ht="15" spans="2:13">
       <c r="B15" s="5"/>
-      <c r="C15" s="64"/>
-      <c r="D15" s="65"/>
-      <c r="E15" s="82" t="s">
+      <c r="C15" s="73"/>
+      <c r="D15" s="74"/>
+      <c r="E15" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="83" t="s">
-        <v>25</v>
-      </c>
-      <c r="G15" s="84" t="s">
-        <v>25</v>
-      </c>
-      <c r="H15" s="89" t="s">
-        <v>25</v>
-      </c>
-      <c r="I15" s="89">
+      <c r="F15" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="93" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15" s="98">
         <v>2</v>
       </c>
-      <c r="J15" s="89" t="s">
-        <v>25</v>
-      </c>
-      <c r="K15" s="89" t="s">
-        <v>25</v>
-      </c>
-      <c r="L15" s="89">
-        <v>1</v>
-      </c>
-      <c r="M15" s="92">
+      <c r="J15" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="K15" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="L15" s="98">
+        <v>1</v>
+      </c>
+      <c r="M15" s="101">
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="2:13">
       <c r="B16" s="5"/>
-      <c r="C16" s="66" t="s">
+      <c r="C16" s="75" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="67"/>
-      <c r="E16" s="75" t="s">
+      <c r="D16" s="76"/>
+      <c r="E16" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="76">
+      <c r="F16" s="85">
         <v>0.75</v>
       </c>
-      <c r="G16" s="77">
+      <c r="G16" s="86">
         <v>1.5</v>
       </c>
-      <c r="H16" s="88">
+      <c r="H16" s="97">
         <v>5</v>
       </c>
-      <c r="I16" s="88">
+      <c r="I16" s="97">
         <v>5</v>
       </c>
-      <c r="J16" s="78" t="s">
-        <v>25</v>
-      </c>
-      <c r="K16" s="78" t="s">
-        <v>25</v>
-      </c>
-      <c r="L16" s="78" t="s">
-        <v>25</v>
-      </c>
-      <c r="M16" s="90" t="s">
+      <c r="J16" s="87" t="s">
+        <v>25</v>
+      </c>
+      <c r="K16" s="87" t="s">
+        <v>25</v>
+      </c>
+      <c r="L16" s="87" t="s">
+        <v>25</v>
+      </c>
+      <c r="M16" s="99" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="17" spans="2:13">
       <c r="B17" s="5"/>
-      <c r="C17" s="62"/>
-      <c r="D17" s="63"/>
-      <c r="E17" s="79" t="s">
+      <c r="C17" s="71"/>
+      <c r="D17" s="72"/>
+      <c r="E17" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="80" t="s">
-        <v>25</v>
-      </c>
-      <c r="G17" s="81" t="s">
-        <v>25</v>
-      </c>
-      <c r="H17" s="78">
+      <c r="F17" s="89" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" s="90" t="s">
+        <v>25</v>
+      </c>
+      <c r="H17" s="87">
         <v>1.8</v>
       </c>
-      <c r="I17" s="78">
-        <v>4</v>
-      </c>
-      <c r="J17" s="78">
+      <c r="I17" s="87">
+        <v>4</v>
+      </c>
+      <c r="J17" s="87">
         <v>1.8</v>
       </c>
-      <c r="K17" s="78">
+      <c r="K17" s="87">
         <v>2.4</v>
       </c>
-      <c r="L17" s="78">
+      <c r="L17" s="87">
         <v>2</v>
       </c>
-      <c r="M17" s="90">
+      <c r="M17" s="99">
         <v>8</v>
       </c>
     </row>
     <row r="18" spans="2:13">
       <c r="B18" s="5"/>
-      <c r="C18" s="62"/>
-      <c r="D18" s="63"/>
-      <c r="E18" s="79" t="s">
-        <v>4</v>
-      </c>
-      <c r="F18" s="80" t="s">
-        <v>25</v>
-      </c>
-      <c r="G18" s="81" t="s">
-        <v>25</v>
-      </c>
-      <c r="H18" s="78" t="s">
-        <v>25</v>
-      </c>
-      <c r="I18" s="78">
+      <c r="C18" s="71"/>
+      <c r="D18" s="72"/>
+      <c r="E18" s="88" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="89" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="90" t="s">
+        <v>25</v>
+      </c>
+      <c r="H18" s="87" t="s">
+        <v>25</v>
+      </c>
+      <c r="I18" s="87">
         <v>16</v>
       </c>
-      <c r="J18" s="78" t="s">
-        <v>25</v>
-      </c>
-      <c r="K18" s="78" t="s">
-        <v>25</v>
-      </c>
-      <c r="L18" s="78">
+      <c r="J18" s="87" t="s">
+        <v>25</v>
+      </c>
+      <c r="K18" s="87" t="s">
+        <v>25</v>
+      </c>
+      <c r="L18" s="87">
         <v>16</v>
       </c>
-      <c r="M18" s="90">
+      <c r="M18" s="99">
         <v>16</v>
       </c>
     </row>
     <row r="19" ht="15" spans="2:13">
       <c r="B19" s="5"/>
-      <c r="C19" s="64"/>
-      <c r="D19" s="65"/>
-      <c r="E19" s="82" t="s">
+      <c r="C19" s="73"/>
+      <c r="D19" s="74"/>
+      <c r="E19" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="83" t="s">
-        <v>25</v>
-      </c>
-      <c r="G19" s="84" t="s">
-        <v>25</v>
-      </c>
-      <c r="H19" s="89" t="s">
-        <v>25</v>
-      </c>
-      <c r="I19" s="89">
+      <c r="F19" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" s="93" t="s">
+        <v>25</v>
+      </c>
+      <c r="H19" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="I19" s="98">
         <v>2</v>
       </c>
-      <c r="J19" s="89" t="s">
-        <v>25</v>
-      </c>
-      <c r="K19" s="89" t="s">
-        <v>25</v>
-      </c>
-      <c r="L19" s="89">
-        <v>1</v>
-      </c>
-      <c r="M19" s="92">
+      <c r="J19" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="K19" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="L19" s="98">
+        <v>1</v>
+      </c>
+      <c r="M19" s="101">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="2:13">
       <c r="B20" s="5"/>
-      <c r="C20" s="66" t="s">
+      <c r="C20" s="75" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="67"/>
-      <c r="E20" s="75" t="s">
+      <c r="D20" s="76"/>
+      <c r="E20" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="76">
+      <c r="F20" s="85">
         <v>3.25</v>
       </c>
-      <c r="G20" s="77">
+      <c r="G20" s="86">
         <v>2.25</v>
       </c>
-      <c r="H20" s="88">
-        <v>1</v>
-      </c>
-      <c r="I20" s="88">
+      <c r="H20" s="97">
+        <v>1</v>
+      </c>
+      <c r="I20" s="97">
         <v>5</v>
       </c>
-      <c r="J20" s="78" t="s">
-        <v>25</v>
-      </c>
-      <c r="K20" s="78" t="s">
-        <v>25</v>
-      </c>
-      <c r="L20" s="78" t="s">
-        <v>25</v>
-      </c>
-      <c r="M20" s="90" t="s">
+      <c r="J20" s="87" t="s">
+        <v>25</v>
+      </c>
+      <c r="K20" s="87" t="s">
+        <v>25</v>
+      </c>
+      <c r="L20" s="87" t="s">
+        <v>25</v>
+      </c>
+      <c r="M20" s="99" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="21" spans="2:13">
       <c r="B21" s="5"/>
-      <c r="C21" s="62"/>
-      <c r="D21" s="63"/>
-      <c r="E21" s="79" t="s">
+      <c r="C21" s="71"/>
+      <c r="D21" s="72"/>
+      <c r="E21" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="F21" s="80" t="s">
-        <v>25</v>
-      </c>
-      <c r="G21" s="81" t="s">
-        <v>25</v>
-      </c>
-      <c r="H21" s="78">
+      <c r="F21" s="89" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" s="90" t="s">
+        <v>25</v>
+      </c>
+      <c r="H21" s="87">
         <v>0.8</v>
       </c>
-      <c r="I21" s="78">
-        <v>1</v>
-      </c>
-      <c r="J21" s="78">
+      <c r="I21" s="87">
+        <v>1</v>
+      </c>
+      <c r="J21" s="87">
         <v>0.8</v>
       </c>
-      <c r="K21" s="78">
+      <c r="K21" s="87">
         <v>0.8</v>
       </c>
-      <c r="L21" s="78">
-        <v>1</v>
-      </c>
-      <c r="M21" s="90">
+      <c r="L21" s="87">
+        <v>1</v>
+      </c>
+      <c r="M21" s="99">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="2:13">
       <c r="B22" s="5"/>
-      <c r="C22" s="62"/>
-      <c r="D22" s="63"/>
-      <c r="E22" s="79" t="s">
-        <v>4</v>
-      </c>
-      <c r="F22" s="80" t="s">
-        <v>25</v>
-      </c>
-      <c r="G22" s="81" t="s">
-        <v>25</v>
-      </c>
-      <c r="H22" s="78" t="s">
-        <v>25</v>
-      </c>
-      <c r="I22" s="78">
-        <v>4</v>
-      </c>
-      <c r="J22" s="78" t="s">
-        <v>25</v>
-      </c>
-      <c r="K22" s="78" t="s">
-        <v>25</v>
-      </c>
-      <c r="L22" s="78">
-        <v>4</v>
-      </c>
-      <c r="M22" s="90">
+      <c r="C22" s="71"/>
+      <c r="D22" s="72"/>
+      <c r="E22" s="88" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" s="89" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="90" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" s="87" t="s">
+        <v>25</v>
+      </c>
+      <c r="I22" s="87">
+        <v>4</v>
+      </c>
+      <c r="J22" s="87" t="s">
+        <v>25</v>
+      </c>
+      <c r="K22" s="87" t="s">
+        <v>25</v>
+      </c>
+      <c r="L22" s="87">
+        <v>4</v>
+      </c>
+      <c r="M22" s="99">
         <v>4</v>
       </c>
     </row>
     <row r="23" ht="15" spans="2:13">
       <c r="B23" s="5"/>
-      <c r="C23" s="64"/>
-      <c r="D23" s="65"/>
-      <c r="E23" s="82" t="s">
+      <c r="C23" s="73"/>
+      <c r="D23" s="74"/>
+      <c r="E23" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="F23" s="83" t="s">
-        <v>25</v>
-      </c>
-      <c r="G23" s="84" t="s">
-        <v>25</v>
-      </c>
-      <c r="H23" s="89" t="s">
-        <v>25</v>
-      </c>
-      <c r="I23" s="89">
-        <v>1</v>
-      </c>
-      <c r="J23" s="89" t="s">
-        <v>25</v>
-      </c>
-      <c r="K23" s="89" t="s">
-        <v>25</v>
-      </c>
-      <c r="L23" s="89">
-        <v>1</v>
-      </c>
-      <c r="M23" s="92">
+      <c r="F23" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" s="93" t="s">
+        <v>25</v>
+      </c>
+      <c r="H23" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="I23" s="98">
+        <v>1</v>
+      </c>
+      <c r="J23" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="K23" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="L23" s="98">
+        <v>1</v>
+      </c>
+      <c r="M23" s="101">
         <v>1</v>
       </c>
     </row>
@@ -3103,16 +3123,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="1.375" customWidth="true"/>
-    <col min="3" max="3" width="7.25" customWidth="true"/>
-    <col min="5" max="5" width="10" customWidth="true"/>
-    <col min="6" max="6" width="5.625" customWidth="true"/>
-    <col min="7" max="7" width="8.25" customWidth="true"/>
-    <col min="8" max="9" width="9.625" customWidth="true"/>
-    <col min="10" max="13" width="12.75" customWidth="true"/>
+    <col min="2" max="2" width="1.375" customWidth="1"/>
+    <col min="3" max="3" width="7.25" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="5.625" customWidth="1"/>
+    <col min="7" max="7" width="8.25" customWidth="1"/>
+    <col min="8" max="9" width="9.625" customWidth="1"/>
+    <col min="10" max="13" width="12.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="9" customHeight="true" spans="6:9">
+    <row r="1" ht="9" customHeight="1" spans="6:9">
       <c r="F1" s="12"/>
       <c r="G1" s="12"/>
       <c r="H1" s="12"/>
@@ -3133,10 +3153,10 @@
       <c r="H2" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
       <c r="M2" s="46"/>
     </row>
     <row r="3" ht="15" spans="3:13">
@@ -3152,16 +3172,16 @@
       <c r="H3" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="55" t="s">
+      <c r="I3" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="55" t="s">
+      <c r="J3" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="55" t="s">
+      <c r="K3" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="55" t="s">
+      <c r="L3" s="58" t="s">
         <v>19</v>
       </c>
       <c r="M3" s="49" t="s">
@@ -3183,22 +3203,22 @@
       <c r="G4" s="50">
         <v>2.75</v>
       </c>
-      <c r="H4" s="20">
+      <c r="H4" s="51">
         <v>1.5</v>
       </c>
-      <c r="I4" s="21">
+      <c r="I4" s="59">
         <v>3</v>
       </c>
-      <c r="J4" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="L4" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="M4" s="31" t="s">
+      <c r="J4" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" s="62" t="s">
         <v>25</v>
       </c>
     </row>
@@ -3209,28 +3229,28 @@
       <c r="E5" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="51" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="52" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="23">
+      <c r="F5" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="54">
         <v>0.8</v>
       </c>
-      <c r="I5" s="24">
-        <v>1</v>
-      </c>
-      <c r="J5" s="24">
+      <c r="I5" s="60">
+        <v>1</v>
+      </c>
+      <c r="J5" s="60">
         <v>0.8</v>
       </c>
-      <c r="K5" s="24">
-        <v>1</v>
-      </c>
-      <c r="L5" s="24">
-        <v>1</v>
-      </c>
-      <c r="M5" s="32">
+      <c r="K5" s="60">
+        <v>1</v>
+      </c>
+      <c r="L5" s="60">
+        <v>1</v>
+      </c>
+      <c r="M5" s="63">
         <v>1</v>
       </c>
     </row>
@@ -3241,28 +3261,28 @@
       <c r="E6" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="51" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="52" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" s="24">
-        <v>4</v>
-      </c>
-      <c r="J6" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="K6" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="L6" s="24">
-        <v>4</v>
-      </c>
-      <c r="M6" s="32">
+      <c r="F6" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="54" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="60">
+        <v>4</v>
+      </c>
+      <c r="J6" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" s="60">
+        <v>4</v>
+      </c>
+      <c r="M6" s="63">
         <v>4</v>
       </c>
     </row>
@@ -3276,25 +3296,25 @@
       <c r="F7" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="I7" s="28">
-        <v>1</v>
-      </c>
-      <c r="J7" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="K7" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="L7" s="28">
-        <v>1</v>
-      </c>
-      <c r="M7" s="33">
+      <c r="G7" s="55" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="61">
+        <v>1</v>
+      </c>
+      <c r="J7" s="61" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" s="61" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" s="61">
+        <v>1</v>
+      </c>
+      <c r="M7" s="64">
         <v>1</v>
       </c>
     </row>
@@ -3313,22 +3333,22 @@
       <c r="G8" s="50">
         <v>1.75</v>
       </c>
-      <c r="H8" s="20">
+      <c r="H8" s="51">
         <v>1.5</v>
       </c>
-      <c r="I8" s="21">
-        <v>4</v>
-      </c>
-      <c r="J8" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="K8" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="L8" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="M8" s="31" t="s">
+      <c r="I8" s="59">
+        <v>4</v>
+      </c>
+      <c r="J8" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="L8" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="M8" s="62" t="s">
         <v>25</v>
       </c>
     </row>
@@ -3339,28 +3359,28 @@
       <c r="E9" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="51" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="52" t="s">
-        <v>25</v>
-      </c>
-      <c r="H9" s="23">
+      <c r="F9" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="54">
         <v>1.2</v>
       </c>
-      <c r="I9" s="24">
-        <v>1</v>
-      </c>
-      <c r="J9" s="24">
+      <c r="I9" s="60">
+        <v>1</v>
+      </c>
+      <c r="J9" s="60">
         <v>0.8</v>
       </c>
-      <c r="K9" s="24">
-        <v>1</v>
-      </c>
-      <c r="L9" s="24">
-        <v>1</v>
-      </c>
-      <c r="M9" s="32">
+      <c r="K9" s="60">
+        <v>1</v>
+      </c>
+      <c r="L9" s="60">
+        <v>1</v>
+      </c>
+      <c r="M9" s="63">
         <v>1</v>
       </c>
     </row>
@@ -3371,28 +3391,28 @@
       <c r="E10" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="51" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" s="52" t="s">
-        <v>25</v>
-      </c>
-      <c r="H10" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="I10" s="24">
-        <v>4</v>
-      </c>
-      <c r="J10" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="K10" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="L10" s="24">
-        <v>4</v>
-      </c>
-      <c r="M10" s="32">
+      <c r="F10" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="54" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" s="60">
+        <v>4</v>
+      </c>
+      <c r="J10" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="K10" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="L10" s="60">
+        <v>4</v>
+      </c>
+      <c r="M10" s="63">
         <v>4</v>
       </c>
     </row>
@@ -3406,25 +3426,25 @@
       <c r="F11" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="H11" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="I11" s="28">
-        <v>1</v>
-      </c>
-      <c r="J11" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="K11" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="L11" s="28">
-        <v>1</v>
-      </c>
-      <c r="M11" s="33">
+      <c r="G11" s="55" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" s="61">
+        <v>1</v>
+      </c>
+      <c r="J11" s="61" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11" s="61" t="s">
+        <v>25</v>
+      </c>
+      <c r="L11" s="61">
+        <v>1</v>
+      </c>
+      <c r="M11" s="64">
         <v>1</v>
       </c>
     </row>
@@ -3443,22 +3463,22 @@
       <c r="G12" s="50">
         <v>1.5</v>
       </c>
-      <c r="H12" s="20">
-        <v>4</v>
-      </c>
-      <c r="I12" s="21">
+      <c r="H12" s="51">
+        <v>4</v>
+      </c>
+      <c r="I12" s="59">
         <v>5</v>
       </c>
-      <c r="J12" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="K12" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="L12" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="M12" s="31" t="s">
+      <c r="J12" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="L12" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="M12" s="62" t="s">
         <v>25</v>
       </c>
     </row>
@@ -3469,28 +3489,28 @@
       <c r="E13" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="51" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="52" t="s">
-        <v>25</v>
-      </c>
-      <c r="H13" s="23">
+      <c r="F13" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="54">
         <v>2.2</v>
       </c>
-      <c r="I13" s="24">
-        <v>1</v>
-      </c>
-      <c r="J13" s="24">
+      <c r="I13" s="60">
+        <v>1</v>
+      </c>
+      <c r="J13" s="60">
         <v>1.6</v>
       </c>
-      <c r="K13" s="24">
+      <c r="K13" s="60">
         <v>1.8</v>
       </c>
-      <c r="L13" s="24">
+      <c r="L13" s="60">
         <v>2</v>
       </c>
-      <c r="M13" s="32">
+      <c r="M13" s="63">
         <v>2</v>
       </c>
     </row>
@@ -3501,28 +3521,28 @@
       <c r="E14" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F14" s="51" t="s">
-        <v>25</v>
-      </c>
-      <c r="G14" s="52" t="s">
-        <v>25</v>
-      </c>
-      <c r="H14" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="I14" s="24">
-        <v>4</v>
-      </c>
-      <c r="J14" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="K14" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="L14" s="24">
+      <c r="F14" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14" s="54" t="s">
+        <v>25</v>
+      </c>
+      <c r="I14" s="60">
+        <v>4</v>
+      </c>
+      <c r="J14" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="K14" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="L14" s="60">
         <v>8</v>
       </c>
-      <c r="M14" s="32">
+      <c r="M14" s="63">
         <v>4</v>
       </c>
     </row>
@@ -3536,25 +3556,25 @@
       <c r="F15" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="G15" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="H15" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="I15" s="28">
+      <c r="G15" s="55" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15" s="61">
         <v>2</v>
       </c>
-      <c r="J15" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="K15" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="L15" s="28">
-        <v>1</v>
-      </c>
-      <c r="M15" s="33">
+      <c r="J15" s="61" t="s">
+        <v>25</v>
+      </c>
+      <c r="K15" s="61" t="s">
+        <v>25</v>
+      </c>
+      <c r="L15" s="61">
+        <v>1</v>
+      </c>
+      <c r="M15" s="64">
         <v>2</v>
       </c>
     </row>
@@ -3573,22 +3593,22 @@
       <c r="G16" s="50">
         <v>1.5</v>
       </c>
-      <c r="H16" s="20">
+      <c r="H16" s="51">
         <v>5</v>
       </c>
-      <c r="I16" s="21">
+      <c r="I16" s="59">
         <v>5</v>
       </c>
-      <c r="J16" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="K16" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="L16" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="M16" s="31" t="s">
+      <c r="J16" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="K16" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="L16" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="M16" s="62" t="s">
         <v>25</v>
       </c>
     </row>
@@ -3599,28 +3619,28 @@
       <c r="E17" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="51" t="s">
-        <v>25</v>
-      </c>
-      <c r="G17" s="52" t="s">
-        <v>25</v>
-      </c>
-      <c r="H17" s="23">
+      <c r="F17" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="H17" s="54">
         <v>1.8</v>
       </c>
-      <c r="I17" s="24">
-        <v>4</v>
-      </c>
-      <c r="J17" s="24">
+      <c r="I17" s="60">
+        <v>4</v>
+      </c>
+      <c r="J17" s="60">
         <v>1.8</v>
       </c>
-      <c r="K17" s="24">
+      <c r="K17" s="60">
         <v>2.4</v>
       </c>
-      <c r="L17" s="24">
+      <c r="L17" s="60">
         <v>2</v>
       </c>
-      <c r="M17" s="32">
+      <c r="M17" s="63">
         <v>8</v>
       </c>
     </row>
@@ -3631,28 +3651,28 @@
       <c r="E18" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F18" s="51" t="s">
-        <v>25</v>
-      </c>
-      <c r="G18" s="52" t="s">
-        <v>25</v>
-      </c>
-      <c r="H18" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="I18" s="24">
+      <c r="F18" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="H18" s="54" t="s">
+        <v>25</v>
+      </c>
+      <c r="I18" s="60">
         <v>16</v>
       </c>
-      <c r="J18" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="K18" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="L18" s="24">
+      <c r="J18" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="K18" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="L18" s="60">
         <v>16</v>
       </c>
-      <c r="M18" s="32">
+      <c r="M18" s="63">
         <v>16</v>
       </c>
     </row>
@@ -3666,25 +3686,25 @@
       <c r="F19" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="G19" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="H19" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="I19" s="28">
+      <c r="G19" s="55" t="s">
+        <v>25</v>
+      </c>
+      <c r="H19" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="I19" s="61">
         <v>2</v>
       </c>
-      <c r="J19" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="K19" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="L19" s="28">
-        <v>1</v>
-      </c>
-      <c r="M19" s="33">
+      <c r="J19" s="61" t="s">
+        <v>25</v>
+      </c>
+      <c r="K19" s="61" t="s">
+        <v>25</v>
+      </c>
+      <c r="L19" s="61">
+        <v>1</v>
+      </c>
+      <c r="M19" s="64">
         <v>1</v>
       </c>
     </row>
@@ -3703,22 +3723,22 @@
       <c r="G20" s="50">
         <v>2.25</v>
       </c>
-      <c r="H20" s="20">
-        <v>1</v>
-      </c>
-      <c r="I20" s="21">
+      <c r="H20" s="51">
+        <v>1</v>
+      </c>
+      <c r="I20" s="59">
         <v>5</v>
       </c>
-      <c r="J20" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="K20" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="L20" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="M20" s="31" t="s">
+      <c r="J20" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="K20" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="L20" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="M20" s="62" t="s">
         <v>25</v>
       </c>
     </row>
@@ -3729,28 +3749,28 @@
       <c r="E21" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="F21" s="51" t="s">
-        <v>25</v>
-      </c>
-      <c r="G21" s="52" t="s">
-        <v>25</v>
-      </c>
-      <c r="H21" s="23">
+      <c r="F21" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="H21" s="54">
         <v>0.8</v>
       </c>
-      <c r="I21" s="24">
-        <v>1</v>
-      </c>
-      <c r="J21" s="24">
+      <c r="I21" s="60">
+        <v>1</v>
+      </c>
+      <c r="J21" s="60">
         <v>0.8</v>
       </c>
-      <c r="K21" s="24">
+      <c r="K21" s="60">
         <v>0.8</v>
       </c>
-      <c r="L21" s="24">
-        <v>1</v>
-      </c>
-      <c r="M21" s="32">
+      <c r="L21" s="60">
+        <v>1</v>
+      </c>
+      <c r="M21" s="63">
         <v>1</v>
       </c>
     </row>
@@ -3761,28 +3781,28 @@
       <c r="E22" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F22" s="51" t="s">
-        <v>25</v>
-      </c>
-      <c r="G22" s="52" t="s">
-        <v>25</v>
-      </c>
-      <c r="H22" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="I22" s="24">
-        <v>4</v>
-      </c>
-      <c r="J22" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="K22" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="L22" s="24">
-        <v>4</v>
-      </c>
-      <c r="M22" s="32">
+      <c r="F22" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" s="54" t="s">
+        <v>25</v>
+      </c>
+      <c r="I22" s="60">
+        <v>4</v>
+      </c>
+      <c r="J22" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="K22" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="L22" s="60">
+        <v>4</v>
+      </c>
+      <c r="M22" s="63">
         <v>4</v>
       </c>
     </row>
@@ -3796,25 +3816,25 @@
       <c r="F23" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="G23" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="H23" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="I23" s="28">
-        <v>1</v>
-      </c>
-      <c r="J23" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="K23" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="L23" s="28">
-        <v>1</v>
-      </c>
-      <c r="M23" s="33">
+      <c r="G23" s="55" t="s">
+        <v>25</v>
+      </c>
+      <c r="H23" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="I23" s="61">
+        <v>1</v>
+      </c>
+      <c r="J23" s="61" t="s">
+        <v>25</v>
+      </c>
+      <c r="K23" s="61" t="s">
+        <v>25</v>
+      </c>
+      <c r="L23" s="61">
+        <v>1</v>
+      </c>
+      <c r="M23" s="64">
         <v>1</v>
       </c>
     </row>
@@ -3842,23 +3862,23 @@
   <dimension ref="B1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:D23"/>
+      <selection activeCell="C2" sqref="C2:K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="1.375" customWidth="true"/>
-    <col min="3" max="3" width="7.25" customWidth="true"/>
-    <col min="5" max="5" width="10" customWidth="true"/>
-    <col min="6" max="7" width="9.625" customWidth="true"/>
-    <col min="8" max="11" width="12.75" customWidth="true"/>
+    <col min="2" max="2" width="1.375" customWidth="1"/>
+    <col min="3" max="3" width="7.25" customWidth="1"/>
+    <col min="5" max="5" width="9.875" customWidth="1"/>
+    <col min="6" max="7" width="9.625" customWidth="1"/>
+    <col min="8" max="11" width="12.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="9" customHeight="true" spans="6:7">
+    <row r="1" ht="9" customHeight="1" spans="6:7">
       <c r="F1" s="12"/>
       <c r="G1" s="12"/>
     </row>
-    <row r="2" spans="3:11">
+    <row r="2" ht="15" spans="3:11">
       <c r="C2" s="1" t="s">
         <v>21</v>
       </c>
@@ -3875,7 +3895,7 @@
       <c r="J2" s="15"/>
       <c r="K2" s="29"/>
     </row>
-    <row r="3" spans="3:11">
+    <row r="3" ht="15" spans="3:11">
       <c r="C3" s="3"/>
       <c r="D3" s="4"/>
       <c r="E3" s="16"/>

</xml_diff>